<commit_message>
update astrometry table 40 Eri BC
</commit_message>
<xml_diff>
--- a/40_eridani_BC_orbit/40-eridani-bc-astrometry.xlsx
+++ b/40_eridani_BC_orbit/40-eridani-bc-astrometry.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmcewing/Documents/GitHub/dsw-notebooks/40-eridani-bc-orbit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmcewing/Documents/GitHub/dsw-notebooks/40_eridani_BC_orbit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32A6DF57-E3BF-9F47-96C2-DB45F27A130A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B04CA3F-7399-8B47-9F15-30535B877485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27600" yWindow="7080" windowWidth="28040" windowHeight="17440" xr2:uid="{0126316F-B11E-8E49-9061-6EABF132F2F4}"/>
+    <workbookView xWindow="20360" yWindow="7080" windowWidth="28040" windowHeight="17440" xr2:uid="{0126316F-B11E-8E49-9061-6EABF132F2F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="40-eridani-bc-astrometry" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>ra_eri_b</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t xml:space="preserve">2022-08-19T08:52:20Z </t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>band_eri_b</t>
+  </si>
+  <si>
+    <t>band_eri_c</t>
+  </si>
+  <si>
+    <t>I_c</t>
   </si>
 </sst>
 </file>
@@ -430,146 +442,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F106CF2-3138-4444-97E2-337A0F152439}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="4" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
         <v>63.826661000000001</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-7.6790019999999997</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>6.3E-2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
         <v>63.825536999999997</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>-7.6770959999999997</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0.124</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
         <v>63.826680000000003</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-7.679049</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3.9E-2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
         <v>63.825574000000003</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>-7.6771700000000003</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
         <v>63.826669000000003</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-7.6791239999999998</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
         <v>63.825544000000001</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>-7.6772669999999996</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>3.9E-2</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 40 Eri BC astrometry
</commit_message>
<xml_diff>
--- a/40_eridani_BC_orbit/40-eridani-bc-astrometry.xlsx
+++ b/40_eridani_BC_orbit/40-eridani-bc-astrometry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmcewing/Documents/GitHub/dsw-notebooks/40_eridani_BC_orbit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B04CA3F-7399-8B47-9F15-30535B877485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91DCC48A-D665-CE42-B8C3-8FB3842A613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20360" yWindow="7080" windowWidth="28040" windowHeight="17440" xr2:uid="{0126316F-B11E-8E49-9061-6EABF132F2F4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ra_eri_b</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>I_c</t>
+  </si>
+  <si>
+    <t>datetime_eri_c</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +481,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>

</xml_diff>